<commit_message>
adding base QGS début base citation modification de coquille grace a QGS ajout de la colone citations_autre _avis dans open_metadata pour ouverture de metadata_avis
</commit_message>
<xml_diff>
--- a/data/raw/collected_metadata/metadata_auteur.xlsx
+++ b/data/raw/collected_metadata/metadata_auteur.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://genes-my.sharepoint.com/personal/lmaurice_ensae_fr/Documents/CCNE/Analyse/CCNE/data/raw/collected_metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="562" documentId="14_{4E693A4A-B2EC-460E-A60F-8C84D95B0E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{311AD48A-4704-4C0F-A860-278C4421C6F6}"/>
+  <xr:revisionPtr revIDLastSave="564" documentId="14_{4E693A4A-B2EC-460E-A60F-8C84D95B0E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14500DEE-DAED-448C-A543-FA43E7EBB867}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-940" windowWidth="22620" windowHeight="13500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24820" yWindow="-550" windowWidth="16780" windowHeight="9280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="base" sheetId="1" r:id="rId1"/>
@@ -2268,8 +2268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R283"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A195" workbookViewId="0">
-      <selection activeCell="B208" sqref="B2:B283"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3541,7 +3541,7 @@
         <v>122</v>
       </c>
       <c r="C40" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D40" t="b">
         <v>0</v>
@@ -4809,7 +4809,7 @@
         <v>206</v>
       </c>
       <c r="C80" t="s">
-        <v>80</v>
+        <v>35</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>

</xml_diff>